<commit_message>
dynamic selector for table input
</commit_message>
<xml_diff>
--- a/Second Version/Sales_Order_Entry_Robot_ChrisSanderson_RossMarshall/report.xlsx
+++ b/Second Version/Sales_Order_Entry_Robot_ChrisSanderson_RossMarshall/report.xlsx
@@ -8,6 +8,7 @@
   <x:sheets>
     <x:sheet name="Sheet1" sheetId="2" r:id="rId2"/>
     <x:sheet name="Sheet1 Sample Invoice_32.pdf" sheetId="5" r:id="rId5"/>
+    <x:sheet name="Sheet1 Sample Invoice.pdf" sheetId="7" r:id="rId7"/>
   </x:sheets>
   <x:definedNames/>
   <x:calcPr calcId="125725"/>
@@ -507,4 +508,66 @@
   <x:headerFooter/>
   <x:tableParts count="0"/>
 </x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:D3"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetData>
+    <x:row r="1" spans="1:4">
+      <x:c r="A1" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B1" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C1" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="D1" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:4">
+      <x:c r="A2" s="0" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="B2" s="0" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C2" s="1">
+        <x:v>44943.625</x:v>
+      </x:c>
+      <x:c r="D2" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:4">
+      <x:c r="A3" s="0" t="n">
+        <x:v>100</x:v>
+      </x:c>
+      <x:c r="B3" s="0" t="n">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="C3" s="1">
+        <x:v>44946.5077546296</x:v>
+      </x:c>
+      <x:c r="D3" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
 </file>
</xml_diff>